<commit_message>
All Study material till 21/02
</commit_message>
<xml_diff>
--- a/LeetCode/75_Questions/Leetcode 75 Questions.xlsx
+++ b/LeetCode/75_Questions/Leetcode 75 Questions.xlsx
@@ -1,26 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamelmohsen/Desktop/GooglePrep/LeetCode/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamelmohsen/Desktop/GooglePrep/LeetCode/75_Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B961B04D-45C0-E64A-93B0-C2CE6C94A2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A28B5CC-F5C8-0F45-B720-B9E09CED03F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="249">
   <si>
     <t>Video Solution</t>
   </si>
@@ -743,13 +753,37 @@
   </si>
   <si>
     <t>While and shift left and write</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use split and preorder </t>
+  </si>
+  <si>
+    <t>preorder first is always root</t>
+  </si>
+  <si>
+    <t>use trie and dfs</t>
+  </si>
+  <si>
+    <t>use sorted heap</t>
+  </si>
+  <si>
+    <t>used bucket sort and o(n)</t>
+  </si>
+  <si>
+    <t>use two prQ, one max for small number and one min for large numbers</t>
+  </si>
+  <si>
+    <t>dfs and hash map</t>
+  </si>
+  <si>
+    <t>use topological sort</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -847,6 +881,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -935,10 +975,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -956,8 +997,10 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1176,8 +1219,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="225" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="E23" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1610,7 +1653,9 @@
       <c r="D28" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
@@ -1625,7 +1670,9 @@
       <c r="D29" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
@@ -2180,7 +2227,9 @@
       <c r="D66" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="E66" s="4"/>
+      <c r="E66" s="4" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="67" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
@@ -2210,7 +2259,9 @@
       <c r="D68" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="E68" s="4"/>
+      <c r="E68" s="4" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="69" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
@@ -2300,7 +2351,9 @@
       <c r="D74" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="E74" s="4"/>
+      <c r="E74" s="4" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="75" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
@@ -2315,7 +2368,9 @@
       <c r="D75" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="E75" s="4"/>
+      <c r="E75" s="4" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="76" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
@@ -2330,13 +2385,15 @@
       <c r="D76" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="E76" s="4"/>
+      <c r="E76" s="4" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="77" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="17" t="s">
         <v>237</v>
       </c>
       <c r="C77" s="4" t="s">
@@ -2345,7 +2402,9 @@
       <c r="D77" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="E77" s="4"/>
+      <c r="E77" s="4" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B78" s="16"/>

</xml_diff>